<commit_message>
PsychoPy builder: small updates
</commit_message>
<xml_diff>
--- a/demos/image_names.xlsx
+++ b/demos/image_names.xlsx
@@ -19,13 +19,13 @@
     <t>image_name</t>
   </si>
   <si>
-    <t>1.jpg</t>
+    <t>im1.jpg</t>
   </si>
   <si>
-    <t>3.jpg</t>
+    <t>im2.jpg</t>
   </si>
   <si>
-    <t>2.jpg</t>
+    <t>im3.jpg</t>
   </si>
 </sst>
 </file>
@@ -382,7 +382,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,13 +405,13 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>

</xml_diff>